<commit_message>
Removed NNExploration Class I never used.
</commit_message>
<xml_diff>
--- a/RESULTS/COLLECTED NO ORACLE/COLLECTED NO ORACLE RESULTS/COLLECTED RESULTS MAIN/ICOLOR_NO_ORACLE_COLLECTED_RESULTS.xlsx
+++ b/RESULTS/COLLECTED NO ORACLE/COLLECTED NO ORACLE RESULTS/COLLECTED RESULTS MAIN/ICOLOR_NO_ORACLE_COLLECTED_RESULTS.xlsx
@@ -249,6 +249,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>ICOLOR</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> RANDOM ORACLE</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -796,11 +826,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-230006768"/>
-        <c:axId val="-234698848"/>
+        <c:axId val="1386575872"/>
+        <c:axId val="1386577504"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-230006768"/>
+        <c:axId val="1386575872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -842,7 +872,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-234698848"/>
+        <c:crossAx val="1386577504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -850,7 +880,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-234698848"/>
+        <c:axId val="1386577504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -902,7 +932,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-230006768"/>
+        <c:crossAx val="1386575872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10320,7 +10350,7 @@
   <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R11" sqref="R11"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>